<commit_message>
moved profesor listeners from view to controller
</commit_message>
<xml_diff>
--- a/Stadiu.xlsx
+++ b/Stadiu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ProiectBD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE686B49-D23F-41E6-891E-56D8E794C369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B48EE8-BA92-499D-A2F2-E9137A9537FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2AD0D08-0C75-4993-A55D-85164F365424}"/>
+    <workbookView xWindow="5760" yWindow="3216" windowWidth="17280" windowHeight="8964" xr2:uid="{F2AD0D08-0C75-4993-A55D-85164F365424}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Gestiunea utilizatorilor</t>
   </si>
@@ -702,12 +702,6 @@
   </si>
   <si>
     <t>All done(cu nuante)</t>
-  </si>
-  <si>
-    <t>Paul</t>
-  </si>
-  <si>
-    <t>Cristi</t>
   </si>
   <si>
     <r>
@@ -1017,7 +1011,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1033,12 +1027,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1068,7 +1056,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1113,7 +1101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1127,26 +1115,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
@@ -1157,6 +1131,8 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1479,8 +1455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DC5E8D-E1E2-47F6-A337-8E1044762486}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1493,7 +1469,7 @@
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1501,7 +1477,7 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1509,15 +1485,15 @@
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1528,20 +1504,16 @@
     </row>
     <row r="6" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
-      <c r="C6" s="12" t="s">
-        <v>36</v>
-      </c>
+      <c r="C6" s="13"/>
     </row>
     <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>37</v>
-      </c>
+      <c r="C7" s="14"/>
     </row>
     <row r="8" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1561,32 +1533,32 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1615,26 +1587,26 @@
     </row>
     <row r="23" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="15" t="s">
-        <v>51</v>
+      <c r="A25" s="12" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1650,12 +1622,12 @@
     </row>
     <row r="30" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1674,17 +1646,17 @@
       </c>
     </row>
     <row r="35" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="10" t="s">
-        <v>47</v>
+      <c r="A35" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="11" t="s">
-        <v>46</v>
+      <c r="A36" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1702,53 +1674,53 @@
       </c>
     </row>
     <row r="41" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="10" t="s">
-        <v>43</v>
+      <c r="A42" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="10" t="s">
+    <row r="48" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="10" t="s">
+    <row r="50" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="4" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="10" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
D. O. N. E.
</commit_message>
<xml_diff>
--- a/Stadiu.xlsx
+++ b/Stadiu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ProiectBD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProiectBD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B48EE8-BA92-499D-A2F2-E9137A9537FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8AC513-F997-48C9-AA50-E6EF8FEE7B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3216" windowWidth="17280" windowHeight="8964" xr2:uid="{F2AD0D08-0C75-4993-A55D-85164F365424}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F2AD0D08-0C75-4993-A55D-85164F365424}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1050,13 +1050,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB3B3FF"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1119,9 +1119,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
@@ -1131,8 +1128,11 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1455,17 +1455,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DC5E8D-E1E2-47F6-A337-8E1044762486}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="182.44140625" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" customWidth="1"/>
+    <col min="1" max="1" width="182.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
@@ -1497,228 +1497,228 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="C6" s="13"/>
-    </row>
-    <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="14"/>
-    </row>
-    <row r="8" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+      <c r="C7" s="13"/>
+    </row>
+    <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
     </row>
-    <row r="20" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="12" t="s">
+    <row r="24" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="12" t="s">
+    <row r="25" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
     </row>
-    <row r="40" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>40</v>
       </c>

</xml_diff>